<commit_message>
Ran 100 more epochs
</commit_message>
<xml_diff>
--- a/Training histories, saved models, confusion matrices/Henrique/4 Conv Layers/32-64-128-128/history_model_all_data_4ConvLayers_grayscale_more_ropout_layers_down_2x128.xlsx
+++ b/Training histories, saved models, confusion matrices/Henrique/4 Conv Layers/32-64-128-128/history_model_all_data_4ConvLayers_grayscale_more_ropout_layers_down_2x128.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>3.840463638305664</v>
+        <v>1168621</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2130783200263977</v>
+        <v>0.8701274991035461</v>
       </c>
       <c r="D2" t="n">
-        <v>3.855000734329224</v>
+        <v>3392630.75</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4778467416763306</v>
+        <v>0.8477761745452881</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>23.03553771972656</v>
+        <v>1177070.375</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4163934290409088</v>
+        <v>0.8730783462524414</v>
       </c>
       <c r="D3" t="n">
-        <v>24.13508033752441</v>
+        <v>3309519.5</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6449527740478516</v>
+        <v>0.8568755984306335</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>154.4890594482422</v>
+        <v>1233999.625</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4969034492969513</v>
+        <v>0.8726411461830139</v>
       </c>
       <c r="D4" t="n">
-        <v>124.3604049682617</v>
+        <v>3728810.5</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6911302208900452</v>
+        <v>0.8612126708030701</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>509.14501953125</v>
+        <v>1235190.25</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5643351674079895</v>
+        <v>0.8714753985404968</v>
       </c>
       <c r="D5" t="n">
-        <v>441.4125671386719</v>
+        <v>4275770</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7281231284141541</v>
+        <v>0.8531337976455688</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1323.3486328125</v>
+        <v>1312736.5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6028050780296326</v>
+        <v>0.8753005266189575</v>
       </c>
       <c r="D6" t="n">
-        <v>1183.311889648438</v>
+        <v>4061277.75</v>
       </c>
       <c r="E6" t="n">
-        <v>0.74725741147995</v>
+        <v>0.8551747798919678</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>3461.40673828125</v>
+        <v>1354673.375</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6151912808418274</v>
+        <v>0.874826967716217</v>
       </c>
       <c r="D7" t="n">
-        <v>2558.47412109375</v>
+        <v>4733259.5</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7730249166488647</v>
+        <v>0.8471809029579163</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>6391.0166015625</v>
+        <v>1334935.25</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6489982008934021</v>
+        <v>0.8784335255622864</v>
       </c>
       <c r="D8" t="n">
-        <v>5827.93359375</v>
+        <v>4136780.25</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7443659901618958</v>
+        <v>0.8545794486999512</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +579,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>10132.970703125</v>
+        <v>1258594.875</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6733697652816772</v>
+        <v>0.8832422494888306</v>
       </c>
       <c r="D9" t="n">
-        <v>7328.224609375</v>
+        <v>4482352</v>
       </c>
       <c r="E9" t="n">
-        <v>0.792669415473938</v>
+        <v>0.8687813878059387</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +596,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>16595.931640625</v>
+        <v>1318233.125</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6847723126411438</v>
+        <v>0.8826229572296143</v>
       </c>
       <c r="D10" t="n">
-        <v>15947.4794921875</v>
+        <v>4143385.25</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7848456501960754</v>
+        <v>0.8661450743675232</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>26727.927734375</v>
+        <v>1362073.5</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6935154795646667</v>
+        <v>0.8822586536407471</v>
       </c>
       <c r="D11" t="n">
-        <v>20449.640625</v>
+        <v>5114650</v>
       </c>
       <c r="E11" t="n">
-        <v>0.8040649890899658</v>
+        <v>0.8589165806770325</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +630,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>36138.40625</v>
+        <v>1354764.625</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7133697867393494</v>
+        <v>0.8822222352027893</v>
       </c>
       <c r="D12" t="n">
-        <v>28955.904296875</v>
+        <v>5486689.5</v>
       </c>
       <c r="E12" t="n">
-        <v>0.8044901490211487</v>
+        <v>0.8431839346885681</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +647,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>50783.29296875</v>
+        <v>1399762.125</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7220036387443542</v>
+        <v>0.883060097694397</v>
       </c>
       <c r="D13" t="n">
-        <v>45228.84375</v>
+        <v>4969912.5</v>
       </c>
       <c r="E13" t="n">
-        <v>0.8129943013191223</v>
+        <v>0.8611276745796204</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +664,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>64386.62890625</v>
+        <v>1470116.125</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7317304015159607</v>
+        <v>0.8841165900230408</v>
       </c>
       <c r="D14" t="n">
-        <v>62637.0859375</v>
+        <v>5646795</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8214984536170959</v>
+        <v>0.8635938167572021</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +681,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>75118.90625</v>
+        <v>1611281.625</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7504917979240417</v>
+        <v>0.8798178434371948</v>
       </c>
       <c r="D15" t="n">
-        <v>74184.78125</v>
+        <v>5382843</v>
       </c>
       <c r="E15" t="n">
-        <v>0.8224338889122009</v>
+        <v>0.865975022315979</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>110838.0546875</v>
+        <v>1576643.375</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7407650351524353</v>
+        <v>0.8832786679267883</v>
       </c>
       <c r="D16" t="n">
-        <v>105669.640625</v>
+        <v>5859267.5</v>
       </c>
       <c r="E16" t="n">
-        <v>0.8186070322990417</v>
+        <v>0.8679309487342834</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>124892.3203125</v>
+        <v>1623763.875</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7600364089012146</v>
+        <v>0.8838615417480469</v>
       </c>
       <c r="D17" t="n">
-        <v>124887.6953125</v>
+        <v>5517874.5</v>
       </c>
       <c r="E17" t="n">
-        <v>0.8337443470954895</v>
+        <v>0.8615528345108032</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +732,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>147092.78125</v>
+        <v>1577047</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7660473585128784</v>
+        <v>0.8856830596923828</v>
       </c>
       <c r="D18" t="n">
-        <v>154849.59375</v>
+        <v>5245419</v>
       </c>
       <c r="E18" t="n">
-        <v>0.8320435285568237</v>
+        <v>0.8731184601783752</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>170887.171875</v>
+        <v>1627599.75</v>
       </c>
       <c r="C19" t="n">
-        <v>0.7753369808197021</v>
+        <v>0.8877959847450256</v>
       </c>
       <c r="D19" t="n">
-        <v>206330.015625</v>
+        <v>6443675</v>
       </c>
       <c r="E19" t="n">
-        <v>0.8243047595024109</v>
+        <v>0.8607024550437927</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +766,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>192040.15625</v>
+        <v>1771892.25</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7860109210014343</v>
+        <v>0.8841530084609985</v>
       </c>
       <c r="D20" t="n">
-        <v>224815.171875</v>
+        <v>6431610.5</v>
       </c>
       <c r="E20" t="n">
-        <v>0.8189471960067749</v>
+        <v>0.8581511974334717</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +783,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>227470.46875</v>
+        <v>1717444.75</v>
       </c>
       <c r="C21" t="n">
-        <v>0.7888888716697693</v>
+        <v>0.887103796005249</v>
       </c>
       <c r="D21" t="n">
-        <v>261004.828125</v>
+        <v>6597479.5</v>
       </c>
       <c r="E21" t="n">
-        <v>0.8378263711929321</v>
+        <v>0.8562802672386169</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +800,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>256629.765625</v>
+        <v>1634485.125</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7914025783538818</v>
+        <v>0.8893260359764099</v>
       </c>
       <c r="D22" t="n">
-        <v>324675.78125</v>
+        <v>7220393.5</v>
       </c>
       <c r="E22" t="n">
-        <v>0.8277914524078369</v>
+        <v>0.8603622913360596</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>296735.09375</v>
+        <v>1693061.875</v>
       </c>
       <c r="C23" t="n">
-        <v>0.7974863648414612</v>
+        <v>0.88852459192276</v>
       </c>
       <c r="D23" t="n">
-        <v>352265.65625</v>
+        <v>6984749</v>
       </c>
       <c r="E23" t="n">
-        <v>0.846330463886261</v>
+        <v>0.84650057554245</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +834,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>314000.59375</v>
+        <v>1797259.75</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8033151030540466</v>
+        <v>0.8895081877708435</v>
       </c>
       <c r="D24" t="n">
-        <v>418827.8125</v>
+        <v>6367564</v>
       </c>
       <c r="E24" t="n">
-        <v>0.837486207485199</v>
+        <v>0.8730334043502808</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +851,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>331842.96875</v>
+        <v>1903548.875</v>
       </c>
       <c r="C25" t="n">
-        <v>0.8138797879219055</v>
+        <v>0.8883788585662842</v>
       </c>
       <c r="D25" t="n">
-        <v>452305.4375</v>
+        <v>7286738.5</v>
       </c>
       <c r="E25" t="n">
-        <v>0.8344246745109558</v>
+        <v>0.8631686568260193</v>
       </c>
     </row>
     <row r="26">
@@ -868,16 +868,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>374081.1875</v>
+        <v>1935034.875</v>
       </c>
       <c r="C26" t="n">
-        <v>0.8136247992515564</v>
+        <v>0.8886339068412781</v>
       </c>
       <c r="D26" t="n">
-        <v>529640.0625</v>
+        <v>7620830.5</v>
       </c>
       <c r="E26" t="n">
-        <v>0.8447997570037842</v>
+        <v>0.8581511974334717</v>
       </c>
     </row>
     <row r="27">
@@ -885,16 +885,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>408561.5625</v>
+        <v>1790750.625</v>
       </c>
       <c r="C27" t="n">
-        <v>0.8155191540718079</v>
+        <v>0.8902003765106201</v>
       </c>
       <c r="D27" t="n">
-        <v>535510.4375</v>
+        <v>7382961</v>
       </c>
       <c r="E27" t="n">
-        <v>0.8439493179321289</v>
+        <v>0.858831524848938</v>
       </c>
     </row>
     <row r="28">
@@ -902,16 +902,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>413033.8125</v>
+        <v>1804395.125</v>
       </c>
       <c r="C28" t="n">
-        <v>0.8259380459785461</v>
+        <v>0.891912579536438</v>
       </c>
       <c r="D28" t="n">
-        <v>657231.0625</v>
+        <v>7465400</v>
       </c>
       <c r="E28" t="n">
-        <v>0.8376562595367432</v>
+        <v>0.8571307063102722</v>
       </c>
     </row>
     <row r="29">
@@ -919,16 +919,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>444038.40625</v>
+        <v>1870639.5</v>
       </c>
       <c r="C29" t="n">
-        <v>0.8264116644859314</v>
+        <v>0.8936612010002136</v>
       </c>
       <c r="D29" t="n">
-        <v>717238.75</v>
+        <v>7829695.5</v>
       </c>
       <c r="E29" t="n">
-        <v>0.8486266136169434</v>
+        <v>0.8631686568260193</v>
       </c>
     </row>
     <row r="30">
@@ -936,16 +936,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>497301.1875</v>
+        <v>1895674.75</v>
       </c>
       <c r="C30" t="n">
-        <v>0.8296175003051758</v>
+        <v>0.8937340378761292</v>
       </c>
       <c r="D30" t="n">
-        <v>874353</v>
+        <v>8305516</v>
       </c>
       <c r="E30" t="n">
-        <v>0.8461604118347168</v>
+        <v>0.854409396648407</v>
       </c>
     </row>
     <row r="31">
@@ -953,16 +953,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>529162.75</v>
+        <v>2159064</v>
       </c>
       <c r="C31" t="n">
-        <v>0.8324226140975952</v>
+        <v>0.8913297057151794</v>
       </c>
       <c r="D31" t="n">
-        <v>861574.125</v>
+        <v>8601013</v>
       </c>
       <c r="E31" t="n">
-        <v>0.8425036072731018</v>
+        <v>0.8765200972557068</v>
       </c>
     </row>
     <row r="32">
@@ -970,16 +970,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>513924.03125</v>
+        <v>2105690</v>
       </c>
       <c r="C32" t="n">
-        <v>0.8401092886924744</v>
+        <v>0.8891438841819763</v>
       </c>
       <c r="D32" t="n">
-        <v>927115.6875</v>
+        <v>8222898</v>
       </c>
       <c r="E32" t="n">
-        <v>0.8367208242416382</v>
+        <v>0.8706522583961487</v>
       </c>
     </row>
     <row r="33">
@@ -987,16 +987,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>552363.375</v>
+        <v>2109290.75</v>
       </c>
       <c r="C33" t="n">
-        <v>0.8405829071998596</v>
+        <v>0.8948269486427307</v>
       </c>
       <c r="D33" t="n">
-        <v>1034417.1875</v>
+        <v>9796170</v>
       </c>
       <c r="E33" t="n">
-        <v>0.8483714461326599</v>
+        <v>0.8528786301612854</v>
       </c>
     </row>
     <row r="34">
@@ -1004,16 +1004,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>581116.1875</v>
+        <v>2061394.75</v>
       </c>
       <c r="C34" t="n">
-        <v>0.8394535779953003</v>
+        <v>0.8945355415344238</v>
       </c>
       <c r="D34" t="n">
-        <v>1115927.5</v>
+        <v>9459951</v>
       </c>
       <c r="E34" t="n">
-        <v>0.840802788734436</v>
+        <v>0.8620631098747253</v>
       </c>
     </row>
     <row r="35">
@@ -1021,16 +1021,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>640524.875</v>
+        <v>2256658.75</v>
       </c>
       <c r="C35" t="n">
-        <v>0.8382877707481384</v>
+        <v>0.8926047086715698</v>
       </c>
       <c r="D35" t="n">
-        <v>1075154.5</v>
+        <v>9379352</v>
       </c>
       <c r="E35" t="n">
-        <v>0.8523684144020081</v>
+        <v>0.865975022315979</v>
       </c>
     </row>
     <row r="36">
@@ -1038,16 +1038,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>657636.625</v>
+        <v>2251803</v>
       </c>
       <c r="C36" t="n">
-        <v>0.8467759490013123</v>
+        <v>0.8942804932594299</v>
       </c>
       <c r="D36" t="n">
-        <v>1381544.5</v>
+        <v>8887182</v>
       </c>
       <c r="E36" t="n">
-        <v>0.8372310400009155</v>
+        <v>0.8480312824249268</v>
       </c>
     </row>
     <row r="37">
@@ -1055,16 +1055,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>657002.625</v>
+        <v>2335528.75</v>
       </c>
       <c r="C37" t="n">
-        <v>0.8498724699020386</v>
+        <v>0.8940255045890808</v>
       </c>
       <c r="D37" t="n">
-        <v>1473756.625</v>
+        <v>9482426</v>
       </c>
       <c r="E37" t="n">
-        <v>0.8516030311584473</v>
+        <v>0.866910457611084</v>
       </c>
     </row>
     <row r="38">
@@ -1072,16 +1072,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>729644.0625</v>
+        <v>2389836</v>
       </c>
       <c r="C38" t="n">
-        <v>0.8494353294372559</v>
+        <v>0.8948269486427307</v>
       </c>
       <c r="D38" t="n">
-        <v>1421083</v>
+        <v>9818246</v>
       </c>
       <c r="E38" t="n">
-        <v>0.8510077595710754</v>
+        <v>0.8714176416397095</v>
       </c>
     </row>
     <row r="39">
@@ -1089,16 +1089,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>744428</v>
+        <v>2514349.75</v>
       </c>
       <c r="C39" t="n">
-        <v>0.8514025211334229</v>
+        <v>0.8921311497688293</v>
       </c>
       <c r="D39" t="n">
-        <v>1518417</v>
+        <v>9694167</v>
       </c>
       <c r="E39" t="n">
-        <v>0.8555999398231506</v>
+        <v>0.8352751135826111</v>
       </c>
     </row>
     <row r="40">
@@ -1106,16 +1106,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>755661.5</v>
+        <v>2427501.75</v>
       </c>
       <c r="C40" t="n">
-        <v>0.8600000143051147</v>
+        <v>0.895300567150116</v>
       </c>
       <c r="D40" t="n">
-        <v>1811618.875</v>
+        <v>10486324</v>
       </c>
       <c r="E40" t="n">
-        <v>0.8266859650611877</v>
+        <v>0.8720129132270813</v>
       </c>
     </row>
     <row r="41">
@@ -1123,16 +1123,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>764147.625</v>
+        <v>2450052</v>
       </c>
       <c r="C41" t="n">
-        <v>0.8576684594154358</v>
+        <v>0.8939526677131653</v>
       </c>
       <c r="D41" t="n">
-        <v>1816539.125</v>
+        <v>11326021</v>
       </c>
       <c r="E41" t="n">
-        <v>0.8614678382873535</v>
+        <v>0.8721830248832703</v>
       </c>
     </row>
     <row r="42">
@@ -1140,16 +1140,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>771197.5625</v>
+        <v>2494585.25</v>
       </c>
       <c r="C42" t="n">
-        <v>0.8601821660995483</v>
+        <v>0.8984699249267578</v>
       </c>
       <c r="D42" t="n">
-        <v>1906729.125</v>
+        <v>10652950</v>
       </c>
       <c r="E42" t="n">
-        <v>0.8558551073074341</v>
+        <v>0.8755846619606018</v>
       </c>
     </row>
     <row r="43">
@@ -1157,16 +1157,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>846766.0625</v>
+        <v>2521434.75</v>
       </c>
       <c r="C43" t="n">
-        <v>0.858542799949646</v>
+        <v>0.9007285833358765</v>
       </c>
       <c r="D43" t="n">
-        <v>2076529.75</v>
+        <v>11098179</v>
       </c>
       <c r="E43" t="n">
-        <v>0.8546645045280457</v>
+        <v>0.8663151860237122</v>
       </c>
     </row>
     <row r="44">
@@ -1174,16 +1174,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>901342.4375</v>
+        <v>2573317.5</v>
       </c>
       <c r="C44" t="n">
-        <v>0.8575592041015625</v>
+        <v>0.897777795791626</v>
       </c>
       <c r="D44" t="n">
-        <v>2242206.5</v>
+        <v>13222080</v>
       </c>
       <c r="E44" t="n">
-        <v>0.8192873597145081</v>
+        <v>0.863423764705658</v>
       </c>
     </row>
     <row r="45">
@@ -1191,16 +1191,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>951713</v>
+        <v>2691803.75</v>
       </c>
       <c r="C45" t="n">
-        <v>0.860109269618988</v>
+        <v>0.8944626450538635</v>
       </c>
       <c r="D45" t="n">
-        <v>2251204.25</v>
+        <v>13734012</v>
       </c>
       <c r="E45" t="n">
-        <v>0.8560251593589783</v>
+        <v>0.8476060628890991</v>
       </c>
     </row>
     <row r="46">
@@ -1208,16 +1208,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>1042972.8125</v>
+        <v>2628886.75</v>
       </c>
       <c r="C46" t="n">
-        <v>0.8571949005126953</v>
+        <v>0.8973405957221985</v>
       </c>
       <c r="D46" t="n">
-        <v>2675602</v>
+        <v>12625546</v>
       </c>
       <c r="E46" t="n">
-        <v>0.8641891479492188</v>
+        <v>0.8642741441726685</v>
       </c>
     </row>
     <row r="47">
@@ -1225,16 +1225,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>1085051.125</v>
+        <v>2763600.5</v>
       </c>
       <c r="C47" t="n">
-        <v>0.862440824508667</v>
+        <v>0.89923495054245</v>
       </c>
       <c r="D47" t="n">
-        <v>2733213.5</v>
+        <v>11676720</v>
       </c>
       <c r="E47" t="n">
-        <v>0.8532187938690186</v>
+        <v>0.8736287355422974</v>
       </c>
     </row>
     <row r="48">
@@ -1242,16 +1242,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>1076257</v>
+        <v>2887632.25</v>
       </c>
       <c r="C48" t="n">
-        <v>0.8642987012863159</v>
+        <v>0.897777795791626</v>
       </c>
       <c r="D48" t="n">
-        <v>2670797.75</v>
+        <v>14055616</v>
       </c>
       <c r="E48" t="n">
-        <v>0.853303849697113</v>
+        <v>0.8579811453819275</v>
       </c>
     </row>
     <row r="49">
@@ -1259,16 +1259,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>1080664.25</v>
+        <v>2813690.25</v>
       </c>
       <c r="C49" t="n">
-        <v>0.8699817657470703</v>
+        <v>0.8985792398452759</v>
       </c>
       <c r="D49" t="n">
-        <v>2922754.75</v>
+        <v>13352830</v>
       </c>
       <c r="E49" t="n">
-        <v>0.8665702939033508</v>
+        <v>0.8633387088775635</v>
       </c>
     </row>
     <row r="50">
@@ -1276,16 +1276,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>1089678.375</v>
+        <v>3148175.75</v>
       </c>
       <c r="C50" t="n">
-        <v>0.8683059811592102</v>
+        <v>0.8970127701759338</v>
       </c>
       <c r="D50" t="n">
-        <v>3228013.5</v>
+        <v>15141409</v>
       </c>
       <c r="E50" t="n">
-        <v>0.8316183090209961</v>
+        <v>0.8618080019950867</v>
       </c>
     </row>
     <row r="51">
@@ -1293,16 +1293,866 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>1170646.375</v>
+        <v>3042553.75</v>
       </c>
       <c r="C51" t="n">
-        <v>0.8680874109268188</v>
+        <v>0.8996721506118774</v>
       </c>
       <c r="D51" t="n">
-        <v>3200713</v>
+        <v>16620957</v>
       </c>
       <c r="E51" t="n">
+        <v>0.8556849956512451</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>3187799.25</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.8990163803100586</v>
+      </c>
+      <c r="D52" t="n">
+        <v>16259074</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.8695467114448547</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>3592631.25</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.8939526677131653</v>
+      </c>
+      <c r="D53" t="n">
+        <v>14875541</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.8540692329406738</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>3180797</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.9001821279525757</v>
+      </c>
+      <c r="D54" t="n">
+        <v>14976874</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.8754145503044128</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>3333919</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.9004007577896118</v>
+      </c>
+      <c r="D55" t="n">
+        <v>17445614</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.8753295540809631</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>3598304.25</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.8981420993804932</v>
+      </c>
+      <c r="D56" t="n">
+        <v>20434814</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.8565354347229004</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>3599917.5</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.8988706469535828</v>
+      </c>
+      <c r="D57" t="n">
+        <v>18817028</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.869461715221405</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>3803853.25</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.8997814059257507</v>
+      </c>
+      <c r="D58" t="n">
+        <v>19120764</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.8518581390380859</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>3861950.75</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.8967577219009399</v>
+      </c>
+      <c r="D59" t="n">
+        <v>19874136</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.8519431948661804</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>3460622</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.9015300273895264</v>
+      </c>
+      <c r="D60" t="n">
+        <v>17981356</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.8692065477371216</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>3498923.25</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.9000728726387024</v>
+      </c>
+      <c r="D61" t="n">
+        <v>18083690</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.8584913611412048</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>3526603.25</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.9021857976913452</v>
+      </c>
+      <c r="D62" t="n">
+        <v>19263426</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.8469257354736328</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>3823725.5</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.9020764827728271</v>
+      </c>
+      <c r="D63" t="n">
+        <v>19628714</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.8742240071296692</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>3880895.75</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.8995992541313171</v>
+      </c>
+      <c r="D64" t="n">
+        <v>20298898</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.8674206733703613</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>4109999</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.9019308090209961</v>
+      </c>
+      <c r="D65" t="n">
+        <v>21767004</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.8581511974334717</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>4140552.75</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.9020764827728271</v>
+      </c>
+      <c r="D66" t="n">
+        <v>21277368</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.8610426187515259</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>3972461</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.903788685798645</v>
+      </c>
+      <c r="D67" t="n">
+        <v>24077366</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.8737987875938416</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>4050309.75</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.9050273299217224</v>
+      </c>
+      <c r="D68" t="n">
+        <v>21922300</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.8691215515136719</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>4231836</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.9038980007171631</v>
+      </c>
+      <c r="D69" t="n">
+        <v>21859726</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.8771154284477234</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>4044347.25</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.9079052805900574</v>
+      </c>
+      <c r="D70" t="n">
+        <v>20471776</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.878476083278656</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>4331700.5</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.90418940782547</v>
+      </c>
+      <c r="D71" t="n">
+        <v>25397268</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.880346953868866</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>4898958.5</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.9009471535682678</v>
+      </c>
+      <c r="D72" t="n">
+        <v>25304036</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.8666553497314453</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>4739287</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.901311457157135</v>
+      </c>
+      <c r="D73" t="n">
+        <v>24807672</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.8570456504821777</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>4856270.5</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.9031329751014709</v>
+      </c>
+      <c r="D74" t="n">
+        <v>27090690</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.8697168231010437</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>4952206</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.9040801525115967</v>
+      </c>
+      <c r="D75" t="n">
+        <v>25173560</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.8554298877716064</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>4848064.5</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.9068487882614136</v>
+      </c>
+      <c r="D76" t="n">
+        <v>26698688</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.8709924221038818</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>5114697.5</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.9043351411819458</v>
+      </c>
+      <c r="D77" t="n">
+        <v>25364548</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.8709073662757874</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>5171011</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.9039344191551208</v>
+      </c>
+      <c r="D78" t="n">
+        <v>27220240</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.8629985451698303</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="n">
+        <v>5190625.5</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.9065209627151489</v>
+      </c>
+      <c r="D79" t="n">
+        <v>32256658</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.8560251593589783</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="n">
+        <v>5164585.5</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.9033879637718201</v>
+      </c>
+      <c r="D80" t="n">
+        <v>27722558</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.8817926645278931</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="n">
+        <v>5394444</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.9045537114143372</v>
+      </c>
+      <c r="D81" t="n">
+        <v>30601406</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.8710774779319763</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="n">
+        <v>5383917.5</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.9065937995910645</v>
+      </c>
+      <c r="D82" t="n">
+        <v>27769098</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.8574708700180054</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="n">
+        <v>5429910.5</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.9044444561004639</v>
+      </c>
+      <c r="D83" t="n">
+        <v>28401750</v>
+      </c>
+      <c r="E83" t="n">
         <v>0.8625733256340027</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="n">
+        <v>5603460.5</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.9062294960021973</v>
+      </c>
+      <c r="D84" t="n">
+        <v>33068418</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.8515179753303528</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="n">
+        <v>5926532.5</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.9045537114143372</v>
+      </c>
+      <c r="D85" t="n">
+        <v>34194468</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.866910457611084</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="n">
+        <v>6191258</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.9047723412513733</v>
+      </c>
+      <c r="D86" t="n">
+        <v>36765952</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.8541542887687683</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="n">
+        <v>6226936</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.9055373668670654</v>
+      </c>
+      <c r="D87" t="n">
+        <v>34969260</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.87226802110672</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="n">
+        <v>6030997.5</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.9054280519485474</v>
+      </c>
+      <c r="D88" t="n">
+        <v>36338420</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.854239284992218</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="n">
+        <v>6292932</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.9055737853050232</v>
+      </c>
+      <c r="D89" t="n">
+        <v>32228372</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.8816226124763489</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="n">
+        <v>6063035</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0.908743143081665</v>
+      </c>
+      <c r="D90" t="n">
+        <v>34960280</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.8763500452041626</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="n">
+        <v>6461882</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.9064116477966309</v>
+      </c>
+      <c r="D91" t="n">
+        <v>35534744</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.873883843421936</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="n">
+        <v>6410853.5</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0.9078688621520996</v>
+      </c>
+      <c r="D92" t="n">
+        <v>38804952</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0.879411518573761</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="n">
+        <v>7553169</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0.9059016108512878</v>
+      </c>
+      <c r="D93" t="n">
+        <v>37314200</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.8698018789291382</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="n">
+        <v>6602545</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0.9090710282325745</v>
+      </c>
+      <c r="D94" t="n">
+        <v>36045372</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.8629985451698303</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="n">
+        <v>7068099</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0.9069945216178894</v>
+      </c>
+      <c r="D95" t="n">
+        <v>39502652</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.8745641708374023</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="n">
+        <v>6889075</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0.9068487882614136</v>
+      </c>
+      <c r="D96" t="n">
+        <v>37741796</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.8715876936912537</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="n">
+        <v>7119832</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0.9091439247131348</v>
+      </c>
+      <c r="D97" t="n">
+        <v>46620052</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0.8619780540466309</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="n">
+        <v>7087068</v>
+      </c>
+      <c r="C98" t="n">
+        <v>0.9070309400558472</v>
+      </c>
+      <c r="D98" t="n">
+        <v>44209004</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0.8729484081268311</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="n">
+        <v>7745269</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0.9078688621520996</v>
+      </c>
+      <c r="D99" t="n">
+        <v>43179996</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.8778807520866394</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="n">
+        <v>7486926</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0.9077231287956238</v>
+      </c>
+      <c r="D100" t="n">
+        <v>45437056</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0.8676758408546448</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="n">
+        <v>7758685.5</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0.9075409770011902</v>
+      </c>
+      <c r="D101" t="n">
+        <v>40319676</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.8684411644935608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>